<commit_message>
updated BOM with 3/8 pluming parts
</commit_message>
<xml_diff>
--- a/variations/Camden/V0.2.1/BOM-SPARC-Camden-V0.2.1.xlsx
+++ b/variations/Camden/V0.2.1/BOM-SPARC-Camden-V0.2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Smart-Pack-for-Advanced-Research-and-Control\variations\Camden\V0.2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D88D8EA-A7DC-4D02-A64F-E1AF0B7D9543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A91F73A-B16E-49D3-9A34-C0C5056D6F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="bill_of_materials" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Total Cost</t>
   </si>
@@ -191,45 +191,21 @@
     <t>https://www.digikey.com/en/products/detail/t-global-technology/TG-AH486-150-150-1-0-0/3042048</t>
   </si>
   <si>
-    <t>https://www.grainger.com/product/SPEEDAIRE-Barbed-Hose-Fitting-For-5-6AFL3?opr=ODOH&amp;analytics=FM:Order%20History</t>
-  </si>
-  <si>
     <t>SPEEDAIRE Barbed Hose Fitting: For 5/16 in Hose I.D., Hose Barb x NPT, 5/16 in x 1/4 in Fitting Size</t>
   </si>
   <si>
     <t>Barb fitting</t>
   </si>
   <si>
-    <t>panel mount barb fitting</t>
-  </si>
-  <si>
-    <t>PARKER Barbed Fitting Union: 3/8 in ID x 1/4 in ID Size, Barbed x Barbed, Brass, Bulkhead, Rigid</t>
-  </si>
-  <si>
-    <t>https://www.grainger.com/product/2GUJ7?gucid=N:N:PS:Paid:GGL:CSM-2295:6VHHZD:20500801:APZ_1&amp;gad_source=1&amp;gad_campaignid=21369464100&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19RsajGZF2w-bnZcF3epzS8M4xEHfpDZzsbYfeG9zBIcO2rvHXHFMrFFoaAoNGEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
     <t>Tubing: PVC, 3/8 in Inside Dia, 1/2 in Outside Dia, 5 ft Lg, Clear, Polyester Braid</t>
   </si>
   <si>
-    <t>braded pvc tubming</t>
-  </si>
-  <si>
     <t>https://www.grainger.com/product/Tubing-PVC-742T39?gucid=N:N:PS:Paid:GGL:CSM-2295:K2UWC0:20500801:APZ_1&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=21369463827&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19RsZM3cz01djgGkrXBnkh3m7nPFZOvY62h02uQEeZVQfYnXJ_JFcZpUAaAuKSEALw_wcB</t>
   </si>
   <si>
     <t>hose clamp</t>
   </si>
   <si>
-    <t>https://www.grainger.com/product/Worm-Gear-Hose-Clamp-201-Stainless-5CYY6</t>
-  </si>
-  <si>
-    <t>Worm Gear Hose Clamp: 201 Stainless Steel, Perforated Band, 3/8 in – 7/8 in Clamping Dia, 10 PK</t>
-  </si>
-  <si>
-    <t>panel eathernet</t>
-  </si>
-  <si>
     <t>FINECABLES Connector: Cat5e/Cat6, Industrial, Panel, Female, Phosphor Bronze, IP67, Female</t>
   </si>
   <si>
@@ -278,9 +254,6 @@
     <t>Anderson Power Products 5900-BK</t>
   </si>
   <si>
-    <t>eathernet cable</t>
-  </si>
-  <si>
     <t>https://www.grainger.com/product/5PZR3?gucid=N:N:PS:Paid:GGL:CSM-2295:DDJWUR:20500801:APZ_1&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=21379885351&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19RsbdymUQqUtYnAXBF1774w4jJdCOiHtys_Y9P4gyvz2tfj_8QtqMd1gaAg0mEALw_wcB</t>
   </si>
   <si>
@@ -344,15 +317,6 @@
     <t>https://www.aliexpress.us/item/3256805148780496.html?gatewayAdapt=glo2usa4itemAdapt</t>
   </si>
   <si>
-    <t>https://www.grainger.com/product/AIGNEP-USA-Tee-Nickel-Plated-Brass-1CPF4?opr=ODOH&amp;analytics=FM:Order%20History</t>
-  </si>
-  <si>
-    <t>Tee: Nickel-Plated Brass, 1/4 in x 1/4 in x 1/4 in Fitting Pipe Size, 2 in Overall Lg</t>
-  </si>
-  <si>
-    <t>1/4 in Tee</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/ni/785996-01/15219166</t>
   </si>
   <si>
@@ -402,6 +366,51 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/mg-chemicals/419D-55ML/9657990</t>
+  </si>
+  <si>
+    <t>Ethernet cable</t>
+  </si>
+  <si>
+    <t>braded PVC tubing</t>
+  </si>
+  <si>
+    <t>panel Ethernet</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/Fuel-Injection-Hose-Clamp-5CZC5</t>
+  </si>
+  <si>
+    <t>Fuel Injection Hose Clamp: Zinc-Plated Steel Band, 1/2 in – 9/16 in Dia., SAE # 6, 10 PK</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/SPEEDAIRE-Barbed-Hose-Fitting-For-3-6AFN8</t>
+  </si>
+  <si>
+    <t>tee to thermocouple reducer</t>
+  </si>
+  <si>
+    <t>3/8 in Tee</t>
+  </si>
+  <si>
+    <t>Tee: Red Brass, 3/8 in x 3/8 in x 3/8 in Fitting Pipe Size, Female NPT x Female NPT x Female NPT</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/Tee-Red-Brass-1VEZ1?opr=PDPRRDSP&amp;analytics=dsrrItems_1CPF5</t>
+  </si>
+  <si>
+    <t>Hex Bushing: Brass, 3/8 in x 1/8 in Fitting Pipe Size, Male NPT x Female NPT, Class 150</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/Hex-Bushing-Brass-6AYW6</t>
+  </si>
+  <si>
+    <t>Anchor Coupling: Brass, 3/8 in x 3/8 in Fitting Pipe Size, Male NPT x Female NPT</t>
+  </si>
+  <si>
+    <t>panel mount dual female mpt</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/PARKER-Anchor-Coupling-Brass-13Y869?opr=ODOH&amp;analytics=FM:Order%20History</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -469,6 +478,9 @@
     </xf>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -807,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3A36C-E8CE-4E50-A172-E48E2F9A45A8}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +898,7 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -898,7 +910,7 @@
         <v>9.99</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E36" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E38" si="0">C3*D3</f>
         <v>9.99</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -950,7 +962,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -975,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1000,7 +1012,7 @@
         <v>28</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -1027,10 +1039,10 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1186,54 +1198,54 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6">
-        <v>2.1</v>
+        <v>1.77</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>8.4</v>
+        <v>14.16</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
       </c>
       <c r="D17" s="6">
-        <v>12.03</v>
+        <v>23.66</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>24.06</v>
+        <v>47.32</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -1246,38 +1258,38 @@
         <v>15.02</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="6">
-        <v>21.27</v>
+        <v>12.46</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
-        <v>21.27</v>
+        <v>12.46</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1290,16 +1302,16 @@
         <v>15.13</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -1312,16 +1324,16 @@
         <v>29.3</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -1334,16 +1346,16 @@
         <v>4.09</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -1356,16 +1368,16 @@
         <v>147.52000000000001</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2">
         <v>4</v>
@@ -1378,16 +1390,16 @@
         <v>5.8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -1400,16 +1412,16 @@
         <v>1.46</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -1422,18 +1434,18 @@
         <v>2195</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -1446,16 +1458,16 @@
         <v>99.89</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2">
         <v>10</v>
@@ -1468,16 +1480,16 @@
         <v>69.2</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2">
         <v>2</v>
@@ -1490,16 +1502,16 @@
         <v>145.5</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -1512,18 +1524,18 @@
         <v>41.17</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C31" s="2">
         <v>2</v>
@@ -1536,16 +1548,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -1558,38 +1570,38 @@
         <v>14.65</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2">
         <v>2</v>
       </c>
-      <c r="D33" s="6">
-        <v>6.06</v>
-      </c>
-      <c r="E33" s="6">
-        <f t="shared" si="0"/>
-        <v>12.12</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>102</v>
+      <c r="D33" s="2">
+        <v>9.85</v>
+      </c>
+      <c r="E33" s="2">
+        <f>C33*D33</f>
+        <v>19.7</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -1602,16 +1614,16 @@
         <v>19.989999999999998</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -1624,16 +1636,16 @@
         <v>1.87</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -1646,25 +1658,30 @@
         <v>22.56</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1687,7 +1704,7 @@
       </c>
       <c r="E42" s="6">
         <f>SUM(E2:E41)</f>
-        <v>12460.929999999997</v>
+        <v>12492.919999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1705,33 +1722,32 @@
     <hyperlink ref="F13" r:id="rId11" xr:uid="{7E2805CC-0B04-4DB0-9F38-3741F75A7D1D}"/>
     <hyperlink ref="F14" r:id="rId12" xr:uid="{6AF56708-0BAB-42E8-A3AE-FD431334CF6C}"/>
     <hyperlink ref="F15" r:id="rId13" xr:uid="{F2324ACB-C085-42C4-8640-3C360A4D119E}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{A4430CD5-3F04-4F39-8FC7-418A2C196358}"/>
-    <hyperlink ref="F17" r:id="rId15" xr:uid="{9135126A-24C0-4A12-968F-F14A3B2136F6}"/>
-    <hyperlink ref="F18" r:id="rId16" xr:uid="{36F5D6E3-807C-49A7-8D30-80566D9949D4}"/>
-    <hyperlink ref="F19" r:id="rId17" xr:uid="{5DBEE37C-590D-4F51-A663-823016400D71}"/>
-    <hyperlink ref="F20" r:id="rId18" xr:uid="{1F94BCB9-4D2C-4C92-8BF0-A4FC479E37E8}"/>
-    <hyperlink ref="F21" r:id="rId19" xr:uid="{6624F982-B428-4251-AA28-31179DCD8937}"/>
-    <hyperlink ref="F22" r:id="rId20" xr:uid="{58E2A489-0714-4655-8748-622D874EF6F8}"/>
-    <hyperlink ref="F23" r:id="rId21" xr:uid="{81E87505-E60E-4515-89EA-9361938F7388}"/>
-    <hyperlink ref="F24" r:id="rId22" xr:uid="{EFDA772F-CC83-4998-A756-1FADE307C734}"/>
-    <hyperlink ref="F25" r:id="rId23" xr:uid="{F81462CE-4E7C-4FAB-8A8E-D305901B6FCF}"/>
-    <hyperlink ref="F28" r:id="rId24" xr:uid="{0B3AB74B-6B3E-4207-9645-7AB7D6617AD3}"/>
-    <hyperlink ref="F29" r:id="rId25" xr:uid="{5CF86D47-7D87-4635-9306-B8490C771687}"/>
-    <hyperlink ref="F30" r:id="rId26" display="https://www.digikey.com/en/products/detail/belden-inc/35618-002500/7041945?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22518541616&amp;gbraid=0AAAAADrbLljEBpjA6o11517XtnCbKLnsR&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19Rsa4nb1dzOV49q-F9Xe7dRzLg9fr09jgomA5Q7py5DmHjVBe4NA0heoaAspGEALw_wcB" xr:uid="{A2DDC80C-6F39-4C44-B776-452B7FA8CAC3}"/>
-    <hyperlink ref="F31" r:id="rId27" xr:uid="{71E7E2F7-3EA3-469E-BDBD-A5E1E2E4F347}"/>
-    <hyperlink ref="F32" r:id="rId28" xr:uid="{F2165E25-79D9-4521-9261-0FF86CB8CEB1}"/>
-    <hyperlink ref="F11" r:id="rId29" xr:uid="{2459F536-6BF7-4F95-8ED6-65EBE68E0306}"/>
-    <hyperlink ref="F33" r:id="rId30" xr:uid="{A1AFF2B0-3BCF-4EB1-A5D8-3277D679C9A9}"/>
-    <hyperlink ref="G6" r:id="rId31" xr:uid="{A8C35020-1C53-4073-BE6C-0F6933CB1921}"/>
-    <hyperlink ref="G5" r:id="rId32" xr:uid="{A49999D0-0D24-4148-A259-6949303F3996}"/>
-    <hyperlink ref="G7" r:id="rId33" xr:uid="{D90F92BC-9947-4813-8C28-6009DA178051}"/>
-    <hyperlink ref="F26" r:id="rId34" xr:uid="{F3415021-EB69-4CB6-B212-558D2454FF2B}"/>
-    <hyperlink ref="G26" r:id="rId35" xr:uid="{E4EF5DF5-36DD-4B50-AF25-A19F9CE4857A}"/>
-    <hyperlink ref="G30" r:id="rId36" xr:uid="{5A940B12-DD8E-47F3-8C44-FCBBD353757C}"/>
-    <hyperlink ref="F35" r:id="rId37" display="https://www.digikey.com/en/products/detail/io-audio-technologies/IO-C14SP-63/21379594?gad_source=1&amp;gad_campaignid=22396809060&amp;gbraid=0AAAAADrbLlisC8UtMjpExL2rbCWoG3ieR&amp;gclid=Cj0KCQjw0NPGBhCDARIsAGAzpp2VLlJaqhBiZUHDGRJcszbohHTDT2yecNaX-w7lJU8lPrGXw1UWNiwaAsExEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{4B8089ED-EC5B-48CB-8DCC-6C3B9EB37FA7}"/>
-    <hyperlink ref="F36" r:id="rId38" xr:uid="{E263962D-47C1-49F9-A559-36360176D757}"/>
+    <hyperlink ref="F18" r:id="rId14" xr:uid="{36F5D6E3-807C-49A7-8D30-80566D9949D4}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{1F94BCB9-4D2C-4C92-8BF0-A4FC479E37E8}"/>
+    <hyperlink ref="F21" r:id="rId16" xr:uid="{6624F982-B428-4251-AA28-31179DCD8937}"/>
+    <hyperlink ref="F22" r:id="rId17" xr:uid="{58E2A489-0714-4655-8748-622D874EF6F8}"/>
+    <hyperlink ref="F23" r:id="rId18" xr:uid="{81E87505-E60E-4515-89EA-9361938F7388}"/>
+    <hyperlink ref="F24" r:id="rId19" xr:uid="{EFDA772F-CC83-4998-A756-1FADE307C734}"/>
+    <hyperlink ref="F25" r:id="rId20" xr:uid="{F81462CE-4E7C-4FAB-8A8E-D305901B6FCF}"/>
+    <hyperlink ref="F28" r:id="rId21" xr:uid="{0B3AB74B-6B3E-4207-9645-7AB7D6617AD3}"/>
+    <hyperlink ref="F29" r:id="rId22" xr:uid="{5CF86D47-7D87-4635-9306-B8490C771687}"/>
+    <hyperlink ref="F30" r:id="rId23" display="https://www.digikey.com/en/products/detail/belden-inc/35618-002500/7041945?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22518541616&amp;gbraid=0AAAAADrbLljEBpjA6o11517XtnCbKLnsR&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19Rsa4nb1dzOV49q-F9Xe7dRzLg9fr09jgomA5Q7py5DmHjVBe4NA0heoaAspGEALw_wcB" xr:uid="{A2DDC80C-6F39-4C44-B776-452B7FA8CAC3}"/>
+    <hyperlink ref="F31" r:id="rId24" xr:uid="{71E7E2F7-3EA3-469E-BDBD-A5E1E2E4F347}"/>
+    <hyperlink ref="F32" r:id="rId25" xr:uid="{F2165E25-79D9-4521-9261-0FF86CB8CEB1}"/>
+    <hyperlink ref="F11" r:id="rId26" xr:uid="{2459F536-6BF7-4F95-8ED6-65EBE68E0306}"/>
+    <hyperlink ref="G6" r:id="rId27" xr:uid="{A8C35020-1C53-4073-BE6C-0F6933CB1921}"/>
+    <hyperlink ref="G5" r:id="rId28" xr:uid="{A49999D0-0D24-4148-A259-6949303F3996}"/>
+    <hyperlink ref="G7" r:id="rId29" xr:uid="{D90F92BC-9947-4813-8C28-6009DA178051}"/>
+    <hyperlink ref="F26" r:id="rId30" xr:uid="{F3415021-EB69-4CB6-B212-558D2454FF2B}"/>
+    <hyperlink ref="G26" r:id="rId31" xr:uid="{E4EF5DF5-36DD-4B50-AF25-A19F9CE4857A}"/>
+    <hyperlink ref="G30" r:id="rId32" xr:uid="{5A940B12-DD8E-47F3-8C44-FCBBD353757C}"/>
+    <hyperlink ref="F35" r:id="rId33" display="https://www.digikey.com/en/products/detail/io-audio-technologies/IO-C14SP-63/21379594?gad_source=1&amp;gad_campaignid=22396809060&amp;gbraid=0AAAAADrbLlisC8UtMjpExL2rbCWoG3ieR&amp;gclid=Cj0KCQjw0NPGBhCDARIsAGAzpp2VLlJaqhBiZUHDGRJcszbohHTDT2yecNaX-w7lJU8lPrGXw1UWNiwaAsExEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{4B8089ED-EC5B-48CB-8DCC-6C3B9EB37FA7}"/>
+    <hyperlink ref="F36" r:id="rId34" xr:uid="{E263962D-47C1-49F9-A559-36360176D757}"/>
+    <hyperlink ref="F16" r:id="rId35" xr:uid="{83A27BB2-9C4A-4120-9925-FBAA61079743}"/>
+    <hyperlink ref="F33" r:id="rId36" xr:uid="{1E1A9060-9FD1-40EB-9CB4-035E777CB97F}"/>
+    <hyperlink ref="F17" r:id="rId37" xr:uid="{E3301FAD-92C1-4805-8EF6-30AE4F47746A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId39"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a part to BOM
</commit_message>
<xml_diff>
--- a/variations/Camden/V0.2.1/BOM-SPARC-Camden-V0.2.1.xlsx
+++ b/variations/Camden/V0.2.1/BOM-SPARC-Camden-V0.2.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Smart-Pack-for-Advanced-Research-and-Control\variations\Camden\V0.2.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34105aa9bb97034c/Documents/GitHub/Smart-Pack-for-Advanced-Research-and-Control/variations/Camden/V0.2.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55CFE31-0E94-47CD-986F-B9BE33B0F14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{C55CFE31-0E94-47CD-986F-B9BE33B0F14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EEB18D2-8E1A-440C-9AFF-2DD297FC25F4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
+    <workbookView xWindow="33810" yWindow="3600" windowWidth="21600" windowHeight="11295" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="bill_of_materials" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Total Cost</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>If you have 1 of these, you could get rid of one of the 3/8 barb fittings from the tee to the pipe</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/MORSE-Hole-Saw-5-8-in-Saw-Dia-54HP10</t>
+  </si>
+  <si>
+    <t>Hole Saw 5/8ths</t>
+  </si>
+  <si>
+    <t>MORSE Hole Saw: 5/8 in Saw Dia., 5/6 Teeth per Inch, 1 7/8 in Max. Cutting Dp, 1/2"-20 Thread Size</t>
   </si>
 </sst>
 </file>
@@ -850,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3A36C-E8CE-4E50-A172-E48E2F9A45A8}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,15 +1832,39 @@
         <v>131</v>
       </c>
     </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>23.73</v>
+      </c>
+      <c r="E41">
+        <v>23.73</v>
+      </c>
+    </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="7"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D43" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="6">
-        <f>SUM(E2:E41)</f>
-        <v>12820.939999999997</v>
-      </c>
-      <c r="F42" s="6"/>
+      <c r="E43" s="6">
+        <f>SUM(E3:E42)</f>
+        <v>12762.469999999996</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1874,8 +1907,9 @@
     <hyperlink ref="G17" r:id="rId37" xr:uid="{E3301FAD-92C1-4805-8EF6-30AE4F47746A}"/>
     <hyperlink ref="G38" r:id="rId38" xr:uid="{94087BF9-485B-4DE1-AA9E-568F4259E676}"/>
     <hyperlink ref="G40" r:id="rId39" xr:uid="{6D79D5B6-03CD-4FCF-94AD-8DF566E11950}"/>
+    <hyperlink ref="G42" r:id="rId40" xr:uid="{4D4B67EB-FB71-4CF3-8E3E-A7B9C0AA78D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>